<commit_message>
code cleanup in datastore
</commit_message>
<xml_diff>
--- a/sprints/technical backlog.xlsx
+++ b/sprints/technical backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>ID #</t>
   </si>
@@ -73,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +84,13 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,7 +122,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +427,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,28 +529,35 @@
       </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="3">
         <v>42693</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>42693</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
JSON store updates for Insert()
</commit_message>
<xml_diff>
--- a/sprints/technical backlog.xlsx
+++ b/sprints/technical backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>ID #</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Rollback partial written record when exception thrown</t>
+  </si>
+  <si>
+    <t>Clean up JSON store errors</t>
+  </si>
+  <si>
+    <t>DataStore/_Test12</t>
   </si>
 </sst>
 </file>
@@ -431,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,17 +589,31 @@
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="3">
         <v>42694</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>42697</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
complete JSON data store for Select
</commit_message>
<xml_diff>
--- a/sprints/technical backlog.xlsx
+++ b/sprints/technical backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>ID #</t>
   </si>
@@ -599,20 +599,25 @@
         <v>18</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="3">
         <v>42697</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish up sprint review
</commit_message>
<xml_diff>
--- a/sprints/technical backlog.xlsx
+++ b/sprints/technical backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>ID #</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Start Issues section for bugs</t>
+  </si>
+  <si>
+    <t>Fix Test Scripts bug with echoing test totals</t>
   </si>
 </sst>
 </file>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,6 +657,21 @@
       </c>
       <c r="C13" s="4" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>42708</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on linear index
</commit_message>
<xml_diff>
--- a/sprints/technical backlog.xlsx
+++ b/sprints/technical backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>ID #</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Fix Test Scripts bug with echoing test totals</t>
+  </si>
+  <si>
+    <t>Finish threading Select from CmdLine to DataStore</t>
   </si>
 </sst>
 </file>
@@ -452,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,6 +674,21 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>42720</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>